<commit_message>
screenshots have been added
</commit_message>
<xml_diff>
--- a/usa.xlsx
+++ b/usa.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>label</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>arizona</t>
-  </si>
-  <si>
-    <t>washingtoncity</t>
   </si>
 </sst>
 </file>
@@ -546,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,420 +652,409 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0.45833333333333348</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>0.45833333333333348</v>
+        <v>0.38405405405405407</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B12">
-        <v>0.38405405405405407</v>
+        <v>0.1114285714285714</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13">
-        <v>0.1114285714285714</v>
+        <v>0.2049999999999999</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14">
-        <v>0.2049999999999999</v>
+        <v>0.16850000000000001</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15">
-        <v>0.16850000000000001</v>
+        <v>0.36</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16">
-        <v>0.36</v>
+        <v>0.2811538461538462</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17">
-        <v>0.2811538461538462</v>
+        <v>0.50454545454545441</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18">
-        <v>0.50454545454545441</v>
+        <v>6.294117647058825E-2</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B19">
-        <v>6.294117647058825E-2</v>
+        <v>0.48</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B20">
-        <v>0.48</v>
+        <v>0.1816528925619833</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21">
-        <v>0.1816528925619833</v>
+        <v>0.20714285714285721</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22">
-        <v>0.20714285714285721</v>
+        <v>0.2731578947368421</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B23">
-        <v>0.2731578947368421</v>
+        <v>0.18309523809523801</v>
       </c>
       <c r="C23" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B24">
-        <v>0.18309523809523801</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25">
-        <v>0.22600000000000001</v>
+        <v>7.4761904761904779E-2</v>
       </c>
       <c r="C25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B26">
-        <v>7.4761904761904779E-2</v>
+        <v>0.16061611374407569</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B27">
-        <v>0.16061611374407569</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="C27" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B28">
-        <v>0.34499999999999997</v>
+        <v>0.25369565217391299</v>
       </c>
       <c r="C28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B29">
-        <v>0.25369565217391299</v>
+        <v>0.40195652173913032</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B30">
-        <v>0.40195652173913032</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B31">
-        <v>3.5000000000000003E-2</v>
+        <v>0.16348623853211</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B32">
-        <v>0.16348623853211</v>
+        <v>0.2013888888888889</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B33">
-        <v>0.2013888888888889</v>
+        <v>0.14741935483870969</v>
       </c>
       <c r="C33" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B34">
-        <v>0.14741935483870969</v>
+        <v>0.12851485148514841</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B35">
-        <v>0.12851485148514841</v>
+        <v>0.14038461538461541</v>
       </c>
       <c r="C35" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B36">
-        <v>0.14038461538461541</v>
+        <v>0.48678571428571432</v>
       </c>
       <c r="C36" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B37">
-        <v>0.48678571428571432</v>
+        <v>9.3333333333333338E-2</v>
       </c>
       <c r="C37" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B38">
-        <v>9.3333333333333338E-2</v>
+        <v>0.2991428571428571</v>
       </c>
       <c r="C38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B39">
-        <v>0.2991428571428571</v>
+        <v>0.25532051282051299</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B40">
-        <v>0.25532051282051299</v>
+        <v>9.5000000000000029E-2</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B41">
-        <v>9.5000000000000029E-2</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="C41" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B42">
-        <v>4.7500000000000001E-2</v>
+        <v>0.21212121212121199</v>
       </c>
       <c r="C42" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B43">
-        <v>0.21212121212121199</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B44">
-        <v>0.22600000000000001</v>
+        <v>0.1785714285714286</v>
       </c>
       <c r="C44" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B45">
-        <v>0.1785714285714286</v>
+        <v>7.4499999999999969E-2</v>
       </c>
       <c r="C45" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B46">
-        <v>7.4499999999999969E-2</v>
+        <v>0.1214285714285714</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>56</v>
-      </c>
-      <c r="B47">
-        <v>0.1214285714285714</v>
-      </c>
-      <c r="C47" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>